<commit_message>
partial update - YS
</commit_message>
<xml_diff>
--- a/BIRDSHOT-HEADATA-Alvi/Training-UTS2/results0/model_predictions1.xlsx
+++ b/BIRDSHOT-HEADATA-Alvi/Training-UTS2/results0/model_predictions1.xlsx
@@ -402,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -469,7 +469,7 @@
         <v>1136</v>
       </c>
       <c r="J2">
-        <v>997.8349609375</v>
+        <v>1160.092895507812</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -501,7 +501,7 @@
         <v>986</v>
       </c>
       <c r="J3">
-        <v>995.2394409179688</v>
+        <v>798.57275390625</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -533,7 +533,7 @@
         <v>446</v>
       </c>
       <c r="J4">
-        <v>964.8048706054688</v>
+        <v>453.0560302734375</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -565,7 +565,7 @@
         <v>1312.9</v>
       </c>
       <c r="J5">
-        <v>1007.26708984375</v>
+        <v>1384.345581054688</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -597,7 +597,7 @@
         <v>1060.7</v>
       </c>
       <c r="J6">
-        <v>993.866943359375</v>
+        <v>1046.085083007812</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -629,7 +629,7 @@
         <v>870.7000000000002</v>
       </c>
       <c r="J7">
-        <v>996.8662719726562</v>
+        <v>886.790283203125</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -661,7 +661,7 @@
         <v>1115</v>
       </c>
       <c r="J8">
-        <v>997.760498046875</v>
+        <v>1212.447265625</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -693,7 +693,7 @@
         <v>1038</v>
       </c>
       <c r="J9">
-        <v>989.1304321289062</v>
+        <v>883.7007446289062</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -725,7 +725,7 @@
         <v>547</v>
       </c>
       <c r="J10">
-        <v>977.2677001953125</v>
+        <v>469.638427734375</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -757,71 +757,71 @@
         <v>1447.1</v>
       </c>
       <c r="J11">
-        <v>1004.145446777344</v>
+        <v>1419.657836914062</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G12">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I12">
-        <v>1142</v>
+        <v>864.2</v>
       </c>
       <c r="J12">
-        <v>995.9058837890625</v>
+        <v>922.9663696289062</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I13">
-        <v>800.2</v>
+        <v>1142</v>
       </c>
       <c r="J13">
-        <v>974.9764404296875</v>
+        <v>1161.335571289062</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -829,63 +829,63 @@
         <v>0</v>
       </c>
       <c r="B14">
-        <v>44.99999999999999</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E14">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G14">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="H14">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>839</v>
+        <v>801.2</v>
       </c>
       <c r="J14">
-        <v>989.4609375</v>
+        <v>943.9409790039062</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>20</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="H15">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>644</v>
+        <v>800.2</v>
       </c>
       <c r="J15">
-        <v>996.6790771484375</v>
+        <v>791.9306030273438</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -893,95 +893,95 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>44.99999999999999</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="H16">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I16">
-        <v>899</v>
+        <v>839</v>
       </c>
       <c r="J16">
-        <v>992.177490234375</v>
+        <v>785.9190063476562</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I17">
-        <v>549.0000000000001</v>
+        <v>644</v>
       </c>
       <c r="J17">
-        <v>958.9163208007812</v>
+        <v>867.4951171875</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B18">
         <v>10</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>54.99999999999999</v>
+        <v>75</v>
       </c>
       <c r="H18">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I18">
-        <v>804</v>
+        <v>899</v>
       </c>
       <c r="J18">
-        <v>975.39111328125</v>
+        <v>940.5346069335938</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -989,63 +989,63 @@
         <v>5</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>54.99999999999999</v>
+        <v>45</v>
       </c>
       <c r="H19">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>1164</v>
+        <v>549.0000000000001</v>
       </c>
       <c r="J19">
-        <v>1000.848937988281</v>
+        <v>479.8463745117188</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B20">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>35</v>
+        <v>54.99999999999999</v>
       </c>
       <c r="H20">
         <v>5</v>
       </c>
       <c r="I20">
-        <v>610</v>
+        <v>804</v>
       </c>
       <c r="J20">
-        <v>985.5737915039062</v>
+        <v>850.448974609375</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1053,31 +1053,31 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>54.99999999999999</v>
+      </c>
+      <c r="H21">
         <v>25</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>45</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
       <c r="I21">
-        <v>615</v>
+        <v>1164</v>
       </c>
       <c r="J21">
-        <v>966.5138549804688</v>
+        <v>1257.58544921875</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1085,10 +1085,10 @@
         <v>0</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1100,144 +1100,144 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="H22">
         <v>5</v>
       </c>
       <c r="I22">
-        <v>604</v>
+        <v>610</v>
       </c>
       <c r="J22">
-        <v>977.8693237304688</v>
+        <v>467.3560485839844</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C23">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F23">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H23">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>1219.5</v>
+        <v>615</v>
       </c>
       <c r="J23">
-        <v>995.688232421875</v>
+        <v>621.5987548828125</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D24">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F24">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I24">
-        <v>971.8</v>
+        <v>604</v>
       </c>
       <c r="J24">
-        <v>993.0664672851562</v>
+        <v>494.3451232910156</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B25">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G25">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H25">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I25">
-        <v>1060</v>
+        <v>1219.5</v>
       </c>
       <c r="J25">
-        <v>991.0242919921875</v>
+        <v>1198.732543945312</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G26">
-        <v>54.99999999999999</v>
+        <v>56</v>
       </c>
       <c r="H26">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I26">
-        <v>977</v>
+        <v>938.4</v>
       </c>
       <c r="J26">
-        <v>995.3602905273438</v>
+        <v>1042.053466796875</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1245,31 +1245,31 @@
         <v>4</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E27">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F27">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G27">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H27">
         <v>4</v>
       </c>
       <c r="I27">
-        <v>976.4</v>
+        <v>971.8</v>
       </c>
       <c r="J27">
-        <v>985.927978515625</v>
+        <v>983.0664672851562</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1277,31 +1277,31 @@
         <v>0</v>
       </c>
       <c r="B28">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H28">
         <v>15</v>
       </c>
       <c r="I28">
-        <v>966</v>
+        <v>1060</v>
       </c>
       <c r="J28">
-        <v>991.076416015625</v>
+        <v>1030.712036132812</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1309,31 +1309,31 @@
         <v>0</v>
       </c>
       <c r="B29">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="C29">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29">
-        <v>10</v>
+        <v>54.99999999999999</v>
       </c>
       <c r="H29">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I29">
-        <v>960</v>
+        <v>977</v>
       </c>
       <c r="J29">
-        <v>985.7500610351562</v>
+        <v>959.0427856445312</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1341,31 +1341,31 @@
         <v>4</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>24</v>
+      </c>
+      <c r="F30">
         <v>12</v>
       </c>
-      <c r="E30">
-        <v>20</v>
-      </c>
-      <c r="F30">
-        <v>8</v>
-      </c>
       <c r="G30">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I30">
-        <v>911.2</v>
+        <v>976.4</v>
       </c>
       <c r="J30">
-        <v>983.2412719726562</v>
+        <v>922.9663696289062</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1373,31 +1373,31 @@
         <v>0</v>
       </c>
       <c r="B31">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C31">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="G31">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H31">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I31">
-        <v>1197</v>
+        <v>966</v>
       </c>
       <c r="J31">
-        <v>991.3932495117188</v>
+        <v>1016.0224609375</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1405,95 +1405,95 @@
         <v>0</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="C32">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="H32">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I32">
-        <v>1095.8</v>
+        <v>960</v>
       </c>
       <c r="J32">
-        <v>998.5624389648438</v>
+        <v>1004.695129394531</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B33">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E33">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G33">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="H33">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>832</v>
+        <v>911.2</v>
       </c>
       <c r="J33">
-        <v>987.248779296875</v>
+        <v>837.6876220703125</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B34">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C34">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F34">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I34">
-        <v>897.5</v>
+        <v>1197</v>
       </c>
       <c r="J34">
-        <v>976.7059936523438</v>
+        <v>1111.370361328125</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1501,31 +1501,31 @@
         <v>0</v>
       </c>
       <c r="B35">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C35">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G35">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H35">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="I35">
-        <v>1311</v>
+        <v>1043.6</v>
       </c>
       <c r="J35">
-        <v>1000.688598632812</v>
+        <v>1077.810668945312</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1536,28 +1536,28 @@
         <v>20</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G36">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H36">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I36">
-        <v>1399.7</v>
+        <v>1095.8</v>
       </c>
       <c r="J36">
-        <v>1002.496520996094</v>
+        <v>1077.810668945312</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1565,63 +1565,63 @@
         <v>0</v>
       </c>
       <c r="B37">
-        <v>35.00000000000001</v>
+        <v>10</v>
       </c>
       <c r="C37">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
       <c r="G37">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H37">
         <v>15</v>
       </c>
       <c r="I37">
-        <v>1042</v>
+        <v>832</v>
       </c>
       <c r="J37">
-        <v>986.7547607421875</v>
+        <v>710.4744262695312</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B38">
-        <v>35.00000000000001</v>
+        <v>12</v>
       </c>
       <c r="C38">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G38">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="H38">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I38">
-        <v>974</v>
+        <v>1069.3</v>
       </c>
       <c r="J38">
-        <v>978.3612060546875</v>
+        <v>1168.615844726562</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1629,31 +1629,31 @@
         <v>4</v>
       </c>
       <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
         <v>16</v>
       </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>4</v>
-      </c>
-      <c r="E39">
-        <v>12</v>
-      </c>
       <c r="F39">
         <v>8</v>
       </c>
       <c r="G39">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I39">
-        <v>1079.9</v>
+        <v>897.5</v>
       </c>
       <c r="J39">
-        <v>996.0560302734375</v>
+        <v>916.113525390625</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1661,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="B40">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C40">
         <v>5</v>
@@ -1670,22 +1670,22 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
       <c r="G40">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="H40">
         <v>25</v>
       </c>
       <c r="I40">
-        <v>1504</v>
+        <v>1311</v>
       </c>
       <c r="J40">
-        <v>1006.489685058594</v>
+        <v>1329.581420898438</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1693,31 +1693,31 @@
         <v>0</v>
       </c>
       <c r="B41">
-        <v>44.99999999999999</v>
+        <v>20</v>
       </c>
       <c r="C41">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G41">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="H41">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I41">
-        <v>1044</v>
+        <v>1399.7</v>
       </c>
       <c r="J41">
-        <v>989.4136962890625</v>
+        <v>1337.135131835938</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1725,31 +1725,31 @@
         <v>0</v>
       </c>
       <c r="B42">
-        <v>20</v>
+        <v>35.00000000000001</v>
       </c>
       <c r="C42">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
       <c r="G42">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H42">
         <v>15</v>
       </c>
       <c r="I42">
-        <v>967</v>
+        <v>1042</v>
       </c>
       <c r="J42">
-        <v>985.937255859375</v>
+        <v>1025.56982421875</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1757,10 +1757,10 @@
         <v>0</v>
       </c>
       <c r="B43">
-        <v>40</v>
+        <v>35.00000000000001</v>
       </c>
       <c r="C43">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1778,10 +1778,10 @@
         <v>5</v>
       </c>
       <c r="I43">
-        <v>863</v>
+        <v>974</v>
       </c>
       <c r="J43">
-        <v>980.2838134765625</v>
+        <v>1000.64013671875</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1789,31 +1789,31 @@
         <v>4</v>
       </c>
       <c r="B44">
+        <v>16</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44">
         <v>12</v>
       </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>12</v>
-      </c>
-      <c r="E44">
-        <v>20</v>
-      </c>
       <c r="F44">
         <v>8</v>
       </c>
       <c r="G44">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I44">
-        <v>846.1</v>
+        <v>1079.9</v>
       </c>
       <c r="J44">
-        <v>982.910888671875</v>
+        <v>1046.393432617188</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1821,31 +1821,31 @@
         <v>0</v>
       </c>
       <c r="B45">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C45">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
+        <v>15</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>15</v>
+      </c>
+      <c r="H45">
         <v>25</v>
       </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>50</v>
-      </c>
-      <c r="H45">
-        <v>5</v>
-      </c>
       <c r="I45">
-        <v>660.0000000000001</v>
+        <v>1504</v>
       </c>
       <c r="J45">
-        <v>979.6019287109375</v>
+        <v>1411.892333984375</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1853,7 +1853,7 @@
         <v>0</v>
       </c>
       <c r="B46">
-        <v>35.00000000000001</v>
+        <v>44.99999999999999</v>
       </c>
       <c r="C46">
         <v>15</v>
@@ -1862,150 +1862,150 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H46">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I46">
-        <v>790</v>
+        <v>1044</v>
       </c>
       <c r="J46">
-        <v>994.5612182617188</v>
+        <v>940.2573852539062</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B47">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C47">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E47">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G47">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H47">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I47">
-        <v>895</v>
+        <v>930.4</v>
       </c>
       <c r="J47">
-        <v>984.4868774414062</v>
+        <v>982.7144165039062</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B48">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D48">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F48">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H48">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I48">
-        <v>1069.3</v>
+        <v>967</v>
       </c>
       <c r="J48">
-        <v>1002.259887695312</v>
+        <v>933.4698486328125</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B49">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F49">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="H49">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="I49">
-        <v>1462.7</v>
+        <v>863</v>
       </c>
       <c r="J49">
-        <v>1008.604187011719</v>
+        <v>942.7015991210938</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E50">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G50">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="H50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I50">
-        <v>782</v>
+        <v>846.1</v>
       </c>
       <c r="J50">
-        <v>970.911376953125</v>
+        <v>811.0241088867188</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2013,63 +2013,63 @@
         <v>0</v>
       </c>
       <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
         <v>25</v>
       </c>
-      <c r="C51">
-        <v>10</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>5</v>
-      </c>
       <c r="F51">
         <v>0</v>
       </c>
       <c r="G51">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H51">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="I51">
-        <v>1144</v>
+        <v>660.0000000000001</v>
       </c>
       <c r="J51">
-        <v>996.9381713867188</v>
+        <v>517.3978881835938</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B52">
-        <v>8</v>
+        <v>35.00000000000001</v>
       </c>
       <c r="C52">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D52">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F52">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H52">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="I52">
-        <v>1143.1</v>
+        <v>790</v>
       </c>
       <c r="J52">
-        <v>999.85693359375</v>
+        <v>795.8610229492188</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2077,16 +2077,16 @@
         <v>0</v>
       </c>
       <c r="B53">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C53">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -2095,45 +2095,45 @@
         <v>40</v>
       </c>
       <c r="H53">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I53">
-        <v>621</v>
+        <v>895</v>
       </c>
       <c r="J53">
-        <v>982.881103515625</v>
+        <v>977.529052734375</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B54">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E54">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G54">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54">
-        <v>798</v>
+        <v>791.6</v>
       </c>
       <c r="J54">
-        <v>954.9894409179688</v>
+        <v>811.0241088867188</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2141,63 +2141,63 @@
         <v>0</v>
       </c>
       <c r="B55">
-        <v>44.99999999999999</v>
+        <v>12</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E55">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G55">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="H55">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I55">
-        <v>671</v>
+        <v>906</v>
       </c>
       <c r="J55">
-        <v>992.8853149414062</v>
+        <v>937.4376831054688</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B56">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E56">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G56">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H56">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I56">
-        <v>557</v>
+        <v>1069.3</v>
       </c>
       <c r="J56">
-        <v>983.9008178710938</v>
+        <v>1087.279907226562</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2205,159 +2205,159 @@
         <v>4</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C57">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E57">
         <v>4</v>
       </c>
       <c r="F57">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G57">
         <v>52</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="I57">
-        <v>1062.7</v>
+        <v>1462.7</v>
       </c>
       <c r="J57">
-        <v>982.328369140625</v>
+        <v>1437.751342773438</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B58">
-        <v>55.00000000000001</v>
+        <v>0</v>
       </c>
       <c r="C58">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G58">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="H58">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I58">
-        <v>952</v>
+        <v>950.9</v>
       </c>
       <c r="J58">
-        <v>989.060791015625</v>
+        <v>1078.984741210938</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B59">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D59">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F59">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G59">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I59">
-        <v>953.9</v>
+        <v>782</v>
       </c>
       <c r="J59">
-        <v>992.4949340820312</v>
+        <v>737.0714721679688</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B60">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C60">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
       <c r="E60">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F60">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="H60">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="I60">
-        <v>1160.3</v>
+        <v>1144</v>
       </c>
       <c r="J60">
-        <v>986.59228515625</v>
+        <v>1260.681396484375</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B61">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E61">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G61">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H61">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I61">
-        <v>721</v>
+        <v>1143.1</v>
       </c>
       <c r="J61">
-        <v>995.7085571289062</v>
+        <v>1173.98974609375</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2365,31 +2365,31 @@
         <v>0</v>
       </c>
       <c r="B62">
-        <v>35.00000000000001</v>
+        <v>25</v>
       </c>
       <c r="C62">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
       <c r="E62">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F62">
         <v>0</v>
       </c>
       <c r="G62">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="H62">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I62">
-        <v>462</v>
+        <v>621</v>
       </c>
       <c r="J62">
-        <v>987.2600708007812</v>
+        <v>549.653076171875</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2397,31 +2397,31 @@
         <v>0</v>
       </c>
       <c r="B63">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C63">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="F63">
         <v>0</v>
       </c>
       <c r="G63">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="H63">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I63">
-        <v>986</v>
+        <v>798</v>
       </c>
       <c r="J63">
-        <v>991.9461669921875</v>
+        <v>479.4799194335938</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2429,7 +2429,7 @@
         <v>0</v>
       </c>
       <c r="B64">
-        <v>5</v>
+        <v>44.99999999999999</v>
       </c>
       <c r="C64">
         <v>5</v>
@@ -2438,86 +2438,86 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F64">
         <v>0</v>
       </c>
       <c r="G64">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="H64">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I64">
-        <v>842</v>
+        <v>671</v>
       </c>
       <c r="J64">
-        <v>985.1094360351562</v>
+        <v>708.38525390625</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="F65">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G65">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="H65">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I65">
-        <v>1057.5</v>
+        <v>557</v>
       </c>
       <c r="J65">
-        <v>992.5538940429688</v>
+        <v>462.9757690429688</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E66">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G66">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H66">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I66">
-        <v>1006</v>
+        <v>1062.7</v>
       </c>
       <c r="J66">
-        <v>984.4271850585938</v>
+        <v>1040.14013671875</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2525,31 +2525,31 @@
         <v>0</v>
       </c>
       <c r="B67">
-        <v>4</v>
+        <v>55.00000000000001</v>
       </c>
       <c r="C67">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F67">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="H67">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I67">
-        <v>1019.4</v>
+        <v>952</v>
       </c>
       <c r="J67">
-        <v>995.2478637695312</v>
+        <v>970.3196411132812</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2557,63 +2557,63 @@
         <v>0</v>
       </c>
       <c r="B68">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C68">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E68">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G68">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H68">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I68">
-        <v>931</v>
+        <v>953.9</v>
       </c>
       <c r="J68">
-        <v>989.1365966796875</v>
+        <v>943.9409790039062</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B69">
         <v>12</v>
       </c>
       <c r="C69">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D69">
         <v>0</v>
       </c>
       <c r="E69">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F69">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G69">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="H69">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="I69">
-        <v>1293.4</v>
+        <v>1160.3</v>
       </c>
       <c r="J69">
-        <v>1013.586242675781</v>
+        <v>1042.053466796875</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2624,28 +2624,28 @@
         <v>30</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D70">
         <v>0</v>
       </c>
       <c r="E70">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F70">
         <v>0</v>
       </c>
       <c r="G70">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H70">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I70">
-        <v>620</v>
+        <v>721</v>
       </c>
       <c r="J70">
-        <v>986.7282104492188</v>
+        <v>717.8878173828125</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2653,31 +2653,31 @@
         <v>0</v>
       </c>
       <c r="B71">
-        <v>20</v>
+        <v>35.00000000000001</v>
       </c>
       <c r="C71">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F71">
         <v>0</v>
       </c>
       <c r="G71">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H71">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I71">
-        <v>561</v>
+        <v>462</v>
       </c>
       <c r="J71">
-        <v>996.657470703125</v>
+        <v>605.4000244140625</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -2685,31 +2685,31 @@
         <v>0</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C72">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D72">
         <v>0</v>
       </c>
       <c r="E72">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F72">
         <v>0</v>
       </c>
       <c r="G72">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="H72">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I72">
-        <v>734.0000000000001</v>
+        <v>986</v>
       </c>
       <c r="J72">
-        <v>974.3925170898438</v>
+        <v>934.663818359375</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -2717,95 +2717,95 @@
         <v>0</v>
       </c>
       <c r="B73">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C73">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="E73">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="F73">
         <v>0</v>
       </c>
       <c r="G73">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H73">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I73">
-        <v>1274</v>
+        <v>842</v>
       </c>
       <c r="J73">
-        <v>996.9114379882812</v>
+        <v>689.0300903320312</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B74">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C74">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E74">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G74">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="H74">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I74">
-        <v>1221</v>
+        <v>1057.5</v>
       </c>
       <c r="J74">
-        <v>994.6153564453125</v>
+        <v>975.6275634765625</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C75">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D75">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E75">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F75">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G75">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H75">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I75">
-        <v>1101.1</v>
+        <v>1006</v>
       </c>
       <c r="J75">
-        <v>995.830810546875</v>
+        <v>987.6940307617188</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -2813,31 +2813,31 @@
         <v>0</v>
       </c>
       <c r="B76">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C76">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E76">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G76">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I76">
-        <v>857</v>
+        <v>1019.4</v>
       </c>
       <c r="J76">
-        <v>981.365478515625</v>
+        <v>960.4669799804688</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -2845,63 +2845,63 @@
         <v>0</v>
       </c>
       <c r="B77">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C77">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D77">
         <v>0</v>
       </c>
       <c r="E77">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F77">
         <v>0</v>
       </c>
       <c r="G77">
-        <v>54.99999999999999</v>
+        <v>40</v>
       </c>
       <c r="H77">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I77">
-        <v>620</v>
+        <v>931</v>
       </c>
       <c r="J77">
-        <v>977.2739868164062</v>
+        <v>1034.98291015625</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B78">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D78">
         <v>0</v>
       </c>
       <c r="E78">
+        <v>4</v>
+      </c>
+      <c r="F78">
+        <v>16</v>
+      </c>
+      <c r="G78">
         <v>40</v>
       </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78">
-        <v>45</v>
-      </c>
       <c r="H78">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="I78">
-        <v>1062</v>
+        <v>1293.4</v>
       </c>
       <c r="J78">
-        <v>965.1141967773438</v>
+        <v>1397.289184570312</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -2909,16 +2909,16 @@
         <v>0</v>
       </c>
       <c r="B79">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C79">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="E79">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -2930,42 +2930,42 @@
         <v>5</v>
       </c>
       <c r="I79">
-        <v>854</v>
+        <v>620</v>
       </c>
       <c r="J79">
-        <v>974.055908203125</v>
+        <v>521.9673461914062</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B80">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C80">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D80">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E80">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G80">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H80">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="I80">
-        <v>1098.1</v>
+        <v>561</v>
       </c>
       <c r="J80">
-        <v>1008.544494628906</v>
+        <v>848.9032592773438</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -2973,31 +2973,31 @@
         <v>0</v>
       </c>
       <c r="B81">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C81">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E81">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G81">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="H81">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I81">
-        <v>932</v>
+        <v>945.9</v>
       </c>
       <c r="J81">
-        <v>984.2404174804688</v>
+        <v>1039.290649414062</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3005,10 +3005,10 @@
         <v>0</v>
       </c>
       <c r="B82">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C82">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -3020,16 +3020,16 @@
         <v>0</v>
       </c>
       <c r="G82">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="H82">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I82">
-        <v>829</v>
+        <v>734.0000000000001</v>
       </c>
       <c r="J82">
-        <v>990.4999389648438</v>
+        <v>775.8018798828125</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3037,31 +3037,31 @@
         <v>0</v>
       </c>
       <c r="B83">
+        <v>20</v>
+      </c>
+      <c r="C83">
+        <v>10</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>5</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
         <v>40</v>
       </c>
-      <c r="C83">
+      <c r="H83">
         <v>25</v>
       </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-      <c r="E83">
-        <v>10</v>
-      </c>
-      <c r="F83">
-        <v>0</v>
-      </c>
-      <c r="G83">
-        <v>20</v>
-      </c>
-      <c r="H83">
-        <v>5</v>
-      </c>
       <c r="I83">
-        <v>996</v>
+        <v>1274</v>
       </c>
       <c r="J83">
-        <v>974.6673583984375</v>
+        <v>1250.287719726562</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3069,127 +3069,127 @@
         <v>0</v>
       </c>
       <c r="B84">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C84">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E84">
+        <v>20</v>
+      </c>
+      <c r="F84">
+        <v>20</v>
+      </c>
+      <c r="G84">
+        <v>28</v>
+      </c>
+      <c r="H84">
         <v>12</v>
       </c>
-      <c r="F84">
-        <v>16</v>
-      </c>
-      <c r="G84">
-        <v>32</v>
-      </c>
-      <c r="H84">
-        <v>8</v>
-      </c>
       <c r="I84">
-        <v>1049.1</v>
+        <v>515.8</v>
       </c>
       <c r="J84">
-        <v>1000.81103515625</v>
+        <v>956.7730712890625</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B85">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C85">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D85">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E85">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F85">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G85">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H85">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="I85">
-        <v>1127</v>
+        <v>1221</v>
       </c>
       <c r="J85">
-        <v>998.8834228515625</v>
+        <v>1248.957641601562</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B86">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C86">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D86">
         <v>0</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F86">
         <v>0</v>
       </c>
       <c r="G86">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H86">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I86">
-        <v>1256</v>
+        <v>1180.3</v>
       </c>
       <c r="J86">
-        <v>998.6983032226562</v>
+        <v>1107.569946289062</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B87">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E87">
+        <v>16</v>
+      </c>
+      <c r="F87">
         <v>12</v>
       </c>
-      <c r="F87">
-        <v>4</v>
-      </c>
       <c r="G87">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="H87">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I87">
-        <v>900.6</v>
+        <v>1101.1</v>
       </c>
       <c r="J87">
-        <v>989.74365234375</v>
+        <v>1039.290649414062</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -3197,31 +3197,31 @@
         <v>0</v>
       </c>
       <c r="B88">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C88">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D88">
         <v>0</v>
       </c>
       <c r="E88">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F88">
         <v>0</v>
       </c>
       <c r="G88">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H88">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I88">
-        <v>634</v>
+        <v>857</v>
       </c>
       <c r="J88">
-        <v>991.7113647460938</v>
+        <v>902.0812377929688</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -3229,7 +3229,7 @@
         <v>0</v>
       </c>
       <c r="B89">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C89">
         <v>5</v>
@@ -3238,86 +3238,86 @@
         <v>0</v>
       </c>
       <c r="E89">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F89">
         <v>0</v>
       </c>
       <c r="G89">
-        <v>20</v>
+        <v>54.99999999999999</v>
       </c>
       <c r="H89">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I89">
-        <v>1325</v>
+        <v>620</v>
       </c>
       <c r="J89">
-        <v>1002.888854980469</v>
+        <v>490.7534790039062</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B90">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="D90">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E90">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F90">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="H90">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I90">
-        <v>1070.6</v>
+        <v>1062</v>
       </c>
       <c r="J90">
-        <v>1011.645202636719</v>
+        <v>996.9169311523438</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D91">
         <v>0</v>
       </c>
       <c r="E91">
-        <v>45.00000000000001</v>
+        <v>5</v>
       </c>
       <c r="F91">
         <v>0</v>
       </c>
       <c r="G91">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I91">
-        <v>492</v>
+        <v>854</v>
       </c>
       <c r="J91">
-        <v>951.8457641601562</v>
+        <v>879.1661376953125</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3328,28 +3328,476 @@
         <v>12</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E92">
+        <v>12</v>
+      </c>
+      <c r="F92">
         <v>16</v>
       </c>
-      <c r="F92">
-        <v>8</v>
-      </c>
       <c r="G92">
+        <v>36</v>
+      </c>
+      <c r="H92">
+        <v>12</v>
+      </c>
+      <c r="I92">
+        <v>1098.1</v>
+      </c>
+      <c r="J92">
+        <v>1210.562866210938</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="B93">
+        <v>25</v>
+      </c>
+      <c r="C93">
+        <v>20</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>10</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>35</v>
+      </c>
+      <c r="H93">
+        <v>10</v>
+      </c>
+      <c r="I93">
+        <v>932</v>
+      </c>
+      <c r="J93">
+        <v>976.52685546875</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94">
+        <v>0</v>
+      </c>
+      <c r="B94">
+        <v>30</v>
+      </c>
+      <c r="C94">
+        <v>10</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>5</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>45</v>
+      </c>
+      <c r="H94">
+        <v>10</v>
+      </c>
+      <c r="I94">
+        <v>829</v>
+      </c>
+      <c r="J94">
+        <v>860.8177490234375</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95">
+        <v>0</v>
+      </c>
+      <c r="B95">
+        <v>40</v>
+      </c>
+      <c r="C95">
+        <v>25</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>10</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>20</v>
+      </c>
+      <c r="H95">
+        <v>5</v>
+      </c>
+      <c r="I95">
+        <v>996</v>
+      </c>
+      <c r="J95">
+        <v>1018.384155273438</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96">
+        <v>0</v>
+      </c>
+      <c r="B96">
+        <v>24</v>
+      </c>
+      <c r="C96">
+        <v>8</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>12</v>
+      </c>
+      <c r="F96">
+        <v>16</v>
+      </c>
+      <c r="G96">
+        <v>32</v>
+      </c>
+      <c r="H96">
+        <v>8</v>
+      </c>
+      <c r="I96">
+        <v>1049.1</v>
+      </c>
+      <c r="J96">
+        <v>1066.290893554688</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97">
+        <v>4</v>
+      </c>
+      <c r="B97">
+        <v>32</v>
+      </c>
+      <c r="C97">
+        <v>8</v>
+      </c>
+      <c r="D97">
+        <v>4</v>
+      </c>
+      <c r="E97">
+        <v>4</v>
+      </c>
+      <c r="F97">
+        <v>20</v>
+      </c>
+      <c r="G97">
+        <v>24</v>
+      </c>
+      <c r="H97">
+        <v>4</v>
+      </c>
+      <c r="I97">
+        <v>1127</v>
+      </c>
+      <c r="J97">
+        <v>1133.184814453125</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98">
+        <v>0</v>
+      </c>
+      <c r="B98">
+        <v>24</v>
+      </c>
+      <c r="C98">
+        <v>8</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>12</v>
+      </c>
+      <c r="F98">
+        <v>16</v>
+      </c>
+      <c r="G98">
+        <v>32</v>
+      </c>
+      <c r="H98">
+        <v>8</v>
+      </c>
+      <c r="I98">
+        <v>957.6</v>
+      </c>
+      <c r="J98">
+        <v>1066.290893554688</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99">
+        <v>0</v>
+      </c>
+      <c r="B99">
+        <v>20</v>
+      </c>
+      <c r="C99">
+        <v>10</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>45</v>
+      </c>
+      <c r="H99">
+        <v>25</v>
+      </c>
+      <c r="I99">
+        <v>1256</v>
+      </c>
+      <c r="J99">
+        <v>1305.279174804688</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100">
+        <v>4</v>
+      </c>
+      <c r="B100">
+        <v>40</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>12</v>
+      </c>
+      <c r="F100">
+        <v>4</v>
+      </c>
+      <c r="G100">
+        <v>36</v>
+      </c>
+      <c r="H100">
+        <v>4</v>
+      </c>
+      <c r="I100">
+        <v>900.6</v>
+      </c>
+      <c r="J100">
+        <v>877.2237548828125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101">
+        <v>0</v>
+      </c>
+      <c r="B101">
+        <v>25</v>
+      </c>
+      <c r="C101">
+        <v>5</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>10</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>50</v>
+      </c>
+      <c r="H101">
+        <v>10</v>
+      </c>
+      <c r="I101">
+        <v>634</v>
+      </c>
+      <c r="J101">
+        <v>707.3486938476562</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102">
+        <v>0</v>
+      </c>
+      <c r="B102">
+        <v>40</v>
+      </c>
+      <c r="C102">
+        <v>5</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>15</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>20</v>
+      </c>
+      <c r="H102">
+        <v>20</v>
+      </c>
+      <c r="I102">
+        <v>1325</v>
+      </c>
+      <c r="J102">
+        <v>1382.752807617188</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103">
+        <v>0</v>
+      </c>
+      <c r="B103">
+        <v>16</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>4</v>
+      </c>
+      <c r="E103">
+        <v>20</v>
+      </c>
+      <c r="F103">
+        <v>20</v>
+      </c>
+      <c r="G103">
+        <v>28</v>
+      </c>
+      <c r="H103">
+        <v>12</v>
+      </c>
+      <c r="I103">
+        <v>1070.6</v>
+      </c>
+      <c r="J103">
+        <v>956.7730712890625</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104">
+        <v>5</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>5</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>45.00000000000001</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>45</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104">
+        <v>492</v>
+      </c>
+      <c r="J104">
+        <v>490.5848388671875</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105">
+        <v>4</v>
+      </c>
+      <c r="B105">
+        <v>20</v>
+      </c>
+      <c r="C105">
+        <v>4</v>
+      </c>
+      <c r="D105">
+        <v>4</v>
+      </c>
+      <c r="E105">
+        <v>16</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
         <v>52</v>
       </c>
-      <c r="H92">
-        <v>8</v>
-      </c>
-      <c r="I92">
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105">
+        <v>761.3</v>
+      </c>
+      <c r="J105">
+        <v>791.9306030273438</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106">
+        <v>4</v>
+      </c>
+      <c r="B106">
+        <v>12</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>16</v>
+      </c>
+      <c r="F106">
+        <v>8</v>
+      </c>
+      <c r="G106">
+        <v>52</v>
+      </c>
+      <c r="H106">
+        <v>8</v>
+      </c>
+      <c r="I106">
         <v>1259.2</v>
       </c>
-      <c r="J92">
-        <v>996.6400146484375</v>
+      <c r="J106">
+        <v>1168.61572265625</v>
       </c>
     </row>
   </sheetData>
@@ -3359,7 +3807,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3426,7 +3874,7 @@
         <v>822</v>
       </c>
       <c r="J2">
-        <v>993.5419311523438</v>
+        <v>638.61767578125</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3458,7 +3906,7 @@
         <v>1021.5</v>
       </c>
       <c r="J3">
-        <v>1025.565185546875</v>
+        <v>960.114501953125</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3490,7 +3938,7 @@
         <v>676</v>
       </c>
       <c r="J4">
-        <v>981.4542236328125</v>
+        <v>509.7470397949219</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3522,7 +3970,7 @@
         <v>816</v>
       </c>
       <c r="J5">
-        <v>973.06689453125</v>
+        <v>775.42724609375</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3554,7 +4002,7 @@
         <v>1040</v>
       </c>
       <c r="J6">
-        <v>995.4669799804688</v>
+        <v>868.8445434570312</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3586,39 +4034,39 @@
         <v>333</v>
       </c>
       <c r="J7">
-        <v>936.17431640625</v>
+        <v>505.7286071777344</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8">
-        <v>764</v>
+        <v>949.4</v>
       </c>
       <c r="J8">
-        <v>977.571533203125</v>
+        <v>1046.393432617188</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3629,60 +4077,60 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>54.99999999999999</v>
+        <v>70</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I9">
-        <v>886</v>
+        <v>764</v>
       </c>
       <c r="J9">
-        <v>980.3801879882812</v>
+        <v>738.5125732421875</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>48</v>
+        <v>54.99999999999999</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I10">
-        <v>988.8</v>
+        <v>886</v>
       </c>
       <c r="J10">
-        <v>992.9432373046875</v>
+        <v>870.5496215820312</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3690,127 +4138,127 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F11">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G11">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I11">
-        <v>920.4</v>
+        <v>988.8</v>
       </c>
       <c r="J11">
-        <v>992.4525146484375</v>
+        <v>982.7144165039062</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>35.00000000000001</v>
+        <v>28</v>
       </c>
       <c r="C12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G12">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>892</v>
+        <v>920.4</v>
       </c>
       <c r="J12">
-        <v>970.4581298828125</v>
+        <v>807.5053100585938</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>35.00000000000001</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="H13">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>1476.3</v>
+        <v>892</v>
       </c>
       <c r="J13">
-        <v>998.9532470703125</v>
+        <v>618.732177734375</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="H14">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I14">
-        <v>1581</v>
+        <v>1476.3</v>
       </c>
       <c r="J14">
-        <v>1008.514526367188</v>
+        <v>1290.851318359375</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3818,31 +4266,31 @@
         <v>0</v>
       </c>
       <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
         <v>25</v>
       </c>
-      <c r="C15">
-        <v>10</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>35</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>25</v>
-      </c>
-      <c r="H15">
-        <v>5</v>
-      </c>
       <c r="I15">
-        <v>576</v>
+        <v>1581</v>
       </c>
       <c r="J15">
-        <v>980.021728515625</v>
+        <v>1395.77734375</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -3850,63 +4298,63 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H16">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I16">
-        <v>850</v>
+        <v>576</v>
       </c>
       <c r="J16">
-        <v>994.8283081054688</v>
+        <v>476.1135864257812</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>54.99999999999999</v>
+        <v>40</v>
       </c>
       <c r="H17">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I17">
-        <v>759</v>
+        <v>850</v>
       </c>
       <c r="J17">
-        <v>971.2199096679688</v>
+        <v>849.6123657226562</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -3914,159 +4362,159 @@
         <v>5</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>50</v>
+        <v>54.99999999999999</v>
       </c>
       <c r="H18">
         <v>5</v>
       </c>
       <c r="I18">
-        <v>691</v>
+        <v>759</v>
       </c>
       <c r="J18">
-        <v>973.0507202148438</v>
+        <v>735.9639282226562</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H19">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I19">
-        <v>1276.4</v>
+        <v>691</v>
       </c>
       <c r="J19">
-        <v>993.0390625</v>
+        <v>1011.278503417969</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B20">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I20">
-        <v>646</v>
+        <v>1276.4</v>
       </c>
       <c r="J20">
-        <v>996.3870239257812</v>
+        <v>1078.984741210938</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I21">
-        <v>1097.4</v>
+        <v>646</v>
       </c>
       <c r="J21">
-        <v>979.0780639648438</v>
+        <v>951.5592651367188</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B22">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C22">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="H22">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I22">
-        <v>945</v>
+        <v>1097.4</v>
       </c>
       <c r="J22">
-        <v>979.4877319335938</v>
+        <v>1088.760498046875</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -4074,31 +4522,31 @@
         <v>0</v>
       </c>
       <c r="B23">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C23">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23">
-        <v>863</v>
+        <v>945</v>
       </c>
       <c r="J23">
-        <v>984.5737915039062</v>
+        <v>888.1220703125</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -4106,95 +4554,159 @@
         <v>0</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C24">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I24">
-        <v>569</v>
+        <v>863</v>
       </c>
       <c r="J24">
-        <v>956.8799438476562</v>
+        <v>926.8262939453125</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="H25">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>1161.4</v>
+        <v>569</v>
       </c>
       <c r="J25">
-        <v>999.71337890625</v>
+        <v>449.3078918457031</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G26">
+        <v>52</v>
+      </c>
+      <c r="H26">
+        <v>24</v>
+      </c>
+      <c r="I26">
+        <v>1161.4</v>
+      </c>
+      <c r="J26">
+        <v>1250.791259765625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>16</v>
+      </c>
+      <c r="F27">
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <v>48</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>888.3</v>
+      </c>
+      <c r="J27">
+        <v>916.1135864257812</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
         <v>65</v>
       </c>
-      <c r="H26">
-        <v>5</v>
-      </c>
-      <c r="I26">
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28">
         <v>622</v>
       </c>
-      <c r="J26">
-        <v>979.2896728515625</v>
+      <c r="J28">
+        <v>982.9739990234375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>